<commit_message>
Bug fix on preproc omp
</commit_message>
<xml_diff>
--- a/Performance analysis/LCMR results.xlsx
+++ b/Performance analysis/LCMR results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\domen\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\domen\Google Drive\Unipv\Magistrale\II anno\Project work\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E959B6E-6A82-4ACA-AEBF-64D129B1763E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B12EFE1-A04B-40A2-A1C1-7C94994D5697}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main loop" sheetId="1" r:id="rId1"/>
@@ -2788,8 +2788,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3111,8 +3111,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04C5935A-7C68-4559-81F5-180DEC4A5D1B}">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3195,16 +3195,16 @@
         <v>28.16</v>
       </c>
       <c r="E4" s="2">
-        <v>21.31</v>
+        <v>20.86</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="4">
         <f>D4/E4</f>
-        <v>1.321445330830596</v>
+        <v>1.3499520613614573</v>
       </c>
       <c r="H4" s="4">
         <f>C4/E4</f>
-        <v>0.31722196152041299</v>
+        <v>0.32406519654841803</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -3219,16 +3219,16 @@
         <v>151.54</v>
       </c>
       <c r="E5" s="2">
-        <v>113.93</v>
+        <v>112.02</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="4">
         <f>D5/E5</f>
-        <v>1.3301149828842269</v>
+        <v>1.3527941439028746</v>
       </c>
       <c r="H5" s="4">
         <f>C5/E5</f>
-        <v>0.32230316861230579</v>
+        <v>0.32779860739153721</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -3243,16 +3243,16 @@
         <v>224.98</v>
       </c>
       <c r="E6" s="5">
-        <v>195.5</v>
+        <v>191.4</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="4">
         <f>D6/E6</f>
-        <v>1.1507928388746802</v>
+        <v>1.1754440961337511</v>
       </c>
       <c r="H6" s="4">
         <f>C6/E6</f>
-        <v>0.30618925831202048</v>
+        <v>0.31274817136886102</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -3267,16 +3267,16 @@
         <v>861.21</v>
       </c>
       <c r="E7" s="2">
-        <v>743.74</v>
+        <v>720.07</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="4">
         <f>D7/E7</f>
-        <v>1.1579449807728508</v>
+        <v>1.1960087213743107</v>
       </c>
       <c r="H7" s="4">
         <f>C7/E7</f>
-        <v>0.24536800494796571</v>
+        <v>0.25343369394642185</v>
       </c>
     </row>
   </sheetData>

</xml_diff>